<commit_message>
some fixes in format_excel_file()
</commit_message>
<xml_diff>
--- a/Book1Book1Done.xlsx
+++ b/Book1Book1Done.xlsx
@@ -54,7 +54,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -77,25 +77,91 @@
       </bottom>
       <diagonal/>
     </border>
-    <border/>
+    <border>
+      <left style="thin">
+        <color rgb="009BBB59"/>
+      </left>
+      <right style="thin">
+        <color rgb="009BBB59"/>
+      </right>
+      <top style="thin">
+        <color rgb="009BBB59"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="009BBB59"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="009BBB59"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="009BBB59"/>
+      </right>
+      <top style="thin">
+        <color rgb="009BBB59"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="009BBB59"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="009BBB59"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="009BBB59"/>
+      </right>
+      <top style="thin">
+        <color rgb="009BBB59"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="009BBB59"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="row_style1" xfId="1" hidden="0"/>
-    <cellStyle name="row_style2" xfId="2" hidden="0"/>
+    <cellStyle name="header_style" xfId="1" hidden="0"/>
+    <cellStyle name="row_style1" xfId="2" hidden="0"/>
+    <cellStyle name="row_style2" xfId="3" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -481,210 +547,223 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="16.5" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="15.5" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>D6-173-22</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="4" t="n"/>
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>K84161</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="E1" s="4" t="n"/>
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>KUBE SKRZYNIA 29</t>
         </is>
       </c>
+      <c r="G1" s="4" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>Ilość</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>Wym.A</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>Wym.B</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="5" t="inlineStr">
         <is>
           <t>Typ płyty</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="5" t="inlineStr">
         <is>
           <t>Grubość</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>Tekst oper.2</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="5" t="inlineStr">
         <is>
           <t>Tekst oper.9</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="6" t="n">
         <v>2300</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="6" t="n">
         <v>1164</v>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
         <is>
           <t>40-10-01-D2609MX</t>
         </is>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>1_Rear_wall</t>
         </is>
       </c>
-      <c r="G3" s="3" t="n"/>
+      <c r="G3" s="6" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="5" t="n">
         <v>2500</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="5" t="n">
         <v>580</v>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" s="5" t="inlineStr">
         <is>
           <t>40-18-01-D2609MX</t>
         </is>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr">
         <is>
           <t>2_Side_Wall</t>
         </is>
       </c>
-      <c r="G4" s="2" t="n"/>
+      <c r="G4" s="5" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="6" t="n">
         <v>2500</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="6" t="n">
         <v>580</v>
       </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>40-10-01-D2609MX</t>
         </is>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>2_Side_Wall</t>
         </is>
       </c>
-      <c r="G5" s="3" t="n"/>
+      <c r="G5" s="6" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="5" t="n">
         <v>2500</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="5" t="n">
         <v>580</v>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" s="5" t="inlineStr">
         <is>
           <t>40-18-01-D2609MX</t>
         </is>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="F6" s="2" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>2_Side_Wall</t>
         </is>
       </c>
-      <c r="G6" s="2" t="n"/>
+      <c r="G6" s="5" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="6" t="n">
         <v>2500</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="6" t="n">
         <v>580</v>
       </c>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
         <is>
           <t>40-18-01-D2609MX</t>
         </is>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>2_Side_Wall</t>
         </is>
       </c>
-      <c r="G7" s="3" t="n"/>
+      <c r="G7" s="6" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="5" t="n">
         <v>2500</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="5" t="n">
         <v>580</v>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D8" s="5" t="inlineStr">
         <is>
           <t>40-18-01-D2609MX</t>
         </is>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="F8" s="2" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr">
         <is>
           <t>2_Side_Wall</t>
         </is>
       </c>
-      <c r="G8" s="2" t="n"/>
+      <c r="G8" s="5" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
+ Text oper 10 collumn
</commit_message>
<xml_diff>
--- a/Book1Book1Done.xlsx
+++ b/Book1Book1Done.xlsx
@@ -236,9 +236,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="MyTable" displayName="MyTable" ref="A2:G8" headerRowCount="1">
-  <autoFilter ref="A2:G8"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="MyTable" displayName="MyTable" ref="A2:H8" headerRowCount="1">
+  <autoFilter ref="A2:H8"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Ilość"/>
     <tableColumn id="2" name="Wym.A"/>
     <tableColumn id="3" name="Wym.B"/>
@@ -246,6 +246,7 @@
     <tableColumn id="5" name="Grubość"/>
     <tableColumn id="6" name="Tekst oper.2"/>
     <tableColumn id="7" name="Tekst oper.9"/>
+    <tableColumn id="8" name="Tekst oper.10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -540,7 +541,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,12 +550,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
     <col width="16.5" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
     <col width="15.5" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -576,7 +578,8 @@
           <t>KUBE SKRZYNIA 29</t>
         </is>
       </c>
-      <c r="G1" s="4" t="n"/>
+      <c r="G1" s="3" t="n"/>
+      <c r="H1" s="4" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
@@ -612,6 +615,11 @@
       <c r="G2" s="5" t="inlineStr">
         <is>
           <t>Tekst oper.9</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>Tekst oper.10</t>
         </is>
       </c>
     </row>
@@ -639,6 +647,7 @@
         </is>
       </c>
       <c r="G3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="n">
@@ -664,16 +673,17 @@
         </is>
       </c>
       <c r="G4" s="5" t="n"/>
+      <c r="H4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>2500</v>
+        <v>2530</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>580</v>
+        <v>610</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
@@ -689,16 +699,17 @@
         </is>
       </c>
       <c r="G5" s="6" t="n"/>
+      <c r="H5" s="6" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>2500</v>
+        <v>2530</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>580</v>
+        <v>610</v>
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
@@ -714,16 +725,17 @@
         </is>
       </c>
       <c r="G6" s="5" t="n"/>
+      <c r="H6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>2500</v>
+        <v>2530</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>580</v>
+        <v>610</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
@@ -739,16 +751,17 @@
         </is>
       </c>
       <c r="G7" s="6" t="n"/>
+      <c r="H7" s="6" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>2500</v>
+        <v>2530</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>580</v>
+        <v>610</v>
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
@@ -764,12 +777,13 @@
         </is>
       </c>
       <c r="G8" s="5" t="n"/>
+      <c r="H8" s="5" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>